<commit_message>
test program with google finance support; fixes
</commit_message>
<xml_diff>
--- a/KNMFin/Support Files/Google Finance Mappings.xlsx
+++ b/KNMFin/Support Files/Google Finance Mappings.xlsx
@@ -9,10 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6090" windowHeight="6915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6090" windowHeight="3360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Financial Statement Mappings" sheetId="3" r:id="rId1"/>
+    <sheet name="Summary" sheetId="9" r:id="rId2"/>
+    <sheet name="SoCF" sheetId="6" r:id="rId3"/>
+    <sheet name="Income Statement" sheetId="5" r:id="rId4"/>
+    <sheet name="Balance Sheet" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="141">
   <si>
     <t>Revenue</t>
   </si>
@@ -360,6 +364,93 @@
   </si>
   <si>
     <t>Statement of Cash Flows</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Current Assets</t>
+  </si>
+  <si>
+    <t>Long-Term Assets</t>
+  </si>
+  <si>
+    <t>Total Long-Term Assets</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>Current Liabilities</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Total Long-Term Liabilities</t>
+  </si>
+  <si>
+    <t>Long-Term Liabilities</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Mkt cap</t>
+  </si>
+  <si>
+    <t>358.60B</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Inst. own</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Exchange</t>
+  </si>
+  <si>
+    <t>52 week-Low</t>
+  </si>
+  <si>
+    <t>52 week-High</t>
+  </si>
+  <si>
+    <t>Range-Low</t>
+  </si>
+  <si>
+    <t>Range-High</t>
+  </si>
+  <si>
+    <t>Vol-Day</t>
+  </si>
+  <si>
+    <t>Vol-Avg.</t>
+  </si>
+  <si>
+    <t>Div Amount</t>
+  </si>
+  <si>
+    <t>Div Yield</t>
   </si>
 </sst>
 </file>
@@ -391,7 +482,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -399,13 +490,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A50" sqref="A2:A50"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1586,4 +1699,718 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>